<commit_message>
Updated BackLog for Sprint 2
</commit_message>
<xml_diff>
--- a/Team Project CSE360/src/Product Backlog.xlsx
+++ b/Team Project CSE360/src/Product Backlog.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marqwon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maguti14\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Reroll Dice</t>
   </si>
   <si>
-    <t>Select 3 Pairs of Dice</t>
-  </si>
-  <si>
     <t>Select Dice Pairs to Use In Each Round</t>
   </si>
   <si>
@@ -118,12 +115,24 @@
   </si>
   <si>
     <t>Select starting points for game</t>
+  </si>
+  <si>
+    <t>Pair Dice</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -175,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -190,6 +199,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -475,22 +485,22 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -500,7 +510,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -531,7 +541,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -544,12 +554,18 @@
       <c r="D3" s="7">
         <v>1</v>
       </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -562,14 +578,18 @@
       <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="I4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -582,19 +602,23 @@
       <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="I5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>10</v>
@@ -602,19 +626,23 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="I6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>10</v>
@@ -622,10 +650,14 @@
       <c r="D7" s="7">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="I7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N7" s="7"/>
     </row>
@@ -634,13 +666,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
+      </c>
+      <c r="E8" s="12">
+        <v>3</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="I8" s="7"/>
       <c r="N8" s="7"/>
@@ -650,13 +688,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
+      </c>
+      <c r="E9" s="12">
+        <v>3</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="N9" s="7"/>
     </row>
@@ -665,13 +709,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
+      </c>
+      <c r="E10" s="12">
+        <v>3</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="N10" s="7"/>
     </row>
@@ -680,13 +730,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
+      </c>
+      <c r="E11" s="12">
+        <v>3</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="N11" s="7"/>
     </row>
@@ -695,13 +751,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
+      </c>
+      <c r="E12" s="12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="I12" s="7"/>
       <c r="N12" s="7"/>
@@ -711,13 +773,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
+      </c>
+      <c r="E13" s="12">
+        <v>3</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="N13" s="7"/>
     </row>
@@ -726,13 +794,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="7">
         <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="N14" s="7"/>
     </row>
@@ -741,13 +815,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="7">
         <v>1</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="N15" s="7"/>
     </row>
@@ -756,13 +836,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="7">
         <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>3</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="I16" s="7"/>
       <c r="N16" s="7"/>
@@ -772,13 +858,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
+      </c>
+      <c r="E17" s="12">
+        <v>3</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="N17" s="7"/>
     </row>
@@ -787,13 +879,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="I18" s="7"/>
       <c r="N18" s="7"/>
@@ -803,13 +901,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="7">
         <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="I19" s="7"/>
       <c r="N19" s="7"/>
@@ -819,7 +923,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>10</v>
@@ -827,50 +931,56 @@
       <c r="D20" s="7">
         <v>1</v>
       </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I21" s="7"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I24" s="7"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I27" s="7"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="I29" s="7"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N30" s="7"/>
     </row>
-    <row r="31" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="I31" s="7"/>
       <c r="N31" s="7"/>
     </row>
-    <row r="32" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="N32" s="7"/>
     </row>
-    <row r="34" spans="3:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C34" s="7"/>
     </row>
   </sheetData>

</xml_diff>